<commit_message>
update Nika's compiled file
</commit_message>
<xml_diff>
--- a/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
+++ b/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="9015" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="9015" firstSheet="16" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="key-to-input-workbooks" sheetId="2" r:id="rId1"/>
@@ -26,6 +26,12 @@
     <sheet name="L-curve_11" sheetId="13" r:id="rId12"/>
     <sheet name="L-curve_12" sheetId="14" r:id="rId13"/>
     <sheet name="L-curve_13" sheetId="15" r:id="rId14"/>
+    <sheet name="L-curve_14" sheetId="17" r:id="rId15"/>
+    <sheet name="L-curve_15" sheetId="18" r:id="rId16"/>
+    <sheet name="L-curve_16" sheetId="19" r:id="rId17"/>
+    <sheet name="L-curve_17" sheetId="20" r:id="rId18"/>
+    <sheet name="L-curve_18" sheetId="21" r:id="rId19"/>
+    <sheet name="L-curve_19" sheetId="22" r:id="rId20"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -37,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="48">
   <si>
     <t>Alpha</t>
   </si>
@@ -2103,7 +2109,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C1" sqref="C1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2401,6 +2407,1556 @@
       </c>
       <c r="F17">
         <v>186791</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.68791881699321678</v>
+      </c>
+      <c r="D2">
+        <v>3.9698464399724104E-2</v>
+      </c>
+      <c r="F2">
+        <v>5566</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.68291328948189889</v>
+      </c>
+      <c r="D3">
+        <v>4.9830448795372628E-2</v>
+      </c>
+      <c r="F3">
+        <v>5310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.66999922178973936</v>
+      </c>
+      <c r="D4">
+        <v>9.146424019072931E-2</v>
+      </c>
+      <c r="F4">
+        <v>5263</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.663219935192218</v>
+      </c>
+      <c r="D5">
+        <v>0.13967751302975101</v>
+      </c>
+      <c r="F5">
+        <v>6332</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.66128503274019501</v>
+      </c>
+      <c r="D6">
+        <v>0.16134052218289091</v>
+      </c>
+      <c r="F6">
+        <v>6487</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.65782691362771017</v>
+      </c>
+      <c r="D7">
+        <v>0.21586348922960252</v>
+      </c>
+      <c r="F7">
+        <v>6791</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.64413249194007427</v>
+      </c>
+      <c r="D8">
+        <v>0.70504277161053963</v>
+      </c>
+      <c r="F8">
+        <v>17822</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.63237818210979091</v>
+      </c>
+      <c r="D9">
+        <v>1.4548716020322894</v>
+      </c>
+      <c r="F9">
+        <v>18961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.63072065862920967</v>
+      </c>
+      <c r="D10">
+        <v>1.639967954892958</v>
+      </c>
+      <c r="F10">
+        <v>21611</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.62828544007413567</v>
+      </c>
+      <c r="D11">
+        <v>2.0211646214654162</v>
+      </c>
+      <c r="F11">
+        <v>20395</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.62579499061626109</v>
+      </c>
+      <c r="D12">
+        <v>2.786500222294511</v>
+      </c>
+      <c r="F12">
+        <v>47059</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.62490977615146492</v>
+      </c>
+      <c r="D13">
+        <v>3.4017471297556967</v>
+      </c>
+      <c r="F13">
+        <v>66991</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.6258421582028727</v>
+      </c>
+      <c r="D14">
+        <v>3.3281147958724504</v>
+      </c>
+      <c r="F14">
+        <v>78562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.62573728833487263</v>
+      </c>
+      <c r="D15">
+        <v>3.6880565450585738</v>
+      </c>
+      <c r="F15">
+        <v>37830</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.62490778019384996</v>
+      </c>
+      <c r="D16">
+        <v>5.7223452388503837</v>
+      </c>
+      <c r="F16">
+        <v>175369</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.62539391806691658</v>
+      </c>
+      <c r="D17">
+        <v>6.5119607436099045</v>
+      </c>
+      <c r="F17">
+        <v>83680</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.68866133811885588</v>
+      </c>
+      <c r="D2">
+        <v>4.103946096632214E-2</v>
+      </c>
+      <c r="F2">
+        <v>5156</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.68316556958397945</v>
+      </c>
+      <c r="D3">
+        <v>5.0923159224345926E-2</v>
+      </c>
+      <c r="F3">
+        <v>5543</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.66935298605929394</v>
+      </c>
+      <c r="D4">
+        <v>9.5414621421438361E-2</v>
+      </c>
+      <c r="F4">
+        <v>5496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.66189379308628282</v>
+      </c>
+      <c r="D5">
+        <v>0.14841996241702199</v>
+      </c>
+      <c r="F5">
+        <v>6087</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.6597858664264018</v>
+      </c>
+      <c r="D6">
+        <v>0.17200874319923276</v>
+      </c>
+      <c r="F6">
+        <v>6133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.65612341310338373</v>
+      </c>
+      <c r="D7">
+        <v>0.22968738291395793</v>
+      </c>
+      <c r="F7">
+        <v>7115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.643845695733263</v>
+      </c>
+      <c r="D8">
+        <v>0.63640740628701187</v>
+      </c>
+      <c r="F8">
+        <v>14032</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.63438083747411578</v>
+      </c>
+      <c r="D9">
+        <v>1.3664099638236944</v>
+      </c>
+      <c r="F9">
+        <v>22696</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.63298212190445546</v>
+      </c>
+      <c r="D10">
+        <v>1.522119048485199</v>
+      </c>
+      <c r="F10">
+        <v>18602</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.63097886832687677</v>
+      </c>
+      <c r="D11">
+        <v>1.836863761061734</v>
+      </c>
+      <c r="F11">
+        <v>19602</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.62810388250366245</v>
+      </c>
+      <c r="D12">
+        <v>2.7673844391255344</v>
+      </c>
+      <c r="F12">
+        <v>76993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.62601379842684923</v>
+      </c>
+      <c r="D13">
+        <v>4.291123089667205</v>
+      </c>
+      <c r="F13">
+        <v>58956</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.62507285847650007</v>
+      </c>
+      <c r="D14">
+        <v>5.337544040121057</v>
+      </c>
+      <c r="F14">
+        <v>79730</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.62395088309421176</v>
+      </c>
+      <c r="D15">
+        <v>7.2638274430653533</v>
+      </c>
+      <c r="F15">
+        <v>52263</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.623953542679898</v>
+      </c>
+      <c r="D16">
+        <v>7.263771120766557</v>
+      </c>
+      <c r="F16">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.62196201344626334</v>
+      </c>
+      <c r="D17">
+        <v>14.722421895298639</v>
+      </c>
+      <c r="F17">
+        <v>131896</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.72936953473083099</v>
+      </c>
+      <c r="D2">
+        <v>4.2606717608913255E-2</v>
+      </c>
+      <c r="F2">
+        <v>4941</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.72310207718960506</v>
+      </c>
+      <c r="D3">
+        <v>5.2806815587148906E-2</v>
+      </c>
+      <c r="F3">
+        <v>3064</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.70830394364467963</v>
+      </c>
+      <c r="D4">
+        <v>0.10009237457623489</v>
+      </c>
+      <c r="F4">
+        <v>5085</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.70044237522816699</v>
+      </c>
+      <c r="D5">
+        <v>0.15598037374439538</v>
+      </c>
+      <c r="F5">
+        <v>5885</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.69823434434176612</v>
+      </c>
+      <c r="D6">
+        <v>0.18067777152232453</v>
+      </c>
+      <c r="F6">
+        <v>5836</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.69455083515204175</v>
+      </c>
+      <c r="D7">
+        <v>0.23856418767983434</v>
+      </c>
+      <c r="F7">
+        <v>6307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.68100907496548191</v>
+      </c>
+      <c r="D8">
+        <v>0.69450571674601458</v>
+      </c>
+      <c r="F8">
+        <v>12988</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.67682985858225564</v>
+      </c>
+      <c r="D9">
+        <v>0.98449051145698219</v>
+      </c>
+      <c r="F9">
+        <v>13703</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.67581625068245665</v>
+      </c>
+      <c r="D10">
+        <v>1.0981005998191022</v>
+      </c>
+      <c r="F10">
+        <v>13232</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.67352160709217956</v>
+      </c>
+      <c r="D11">
+        <v>1.4649324749801729</v>
+      </c>
+      <c r="F11">
+        <v>19792</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.6700996735435838</v>
+      </c>
+      <c r="D12">
+        <v>2.5449143699944541</v>
+      </c>
+      <c r="F12">
+        <v>36431</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.66832597304123131</v>
+      </c>
+      <c r="D13">
+        <v>4.2531287818974652</v>
+      </c>
+      <c r="F13">
+        <v>18064</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.66832597304123131</v>
+      </c>
+      <c r="D14">
+        <v>4.2531287818974652</v>
+      </c>
+      <c r="F14">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.66832597304123131</v>
+      </c>
+      <c r="D15">
+        <v>4.2531287818974652</v>
+      </c>
+      <c r="F15">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.66832597304123131</v>
+      </c>
+      <c r="D16">
+        <v>4.2531287818974652</v>
+      </c>
+      <c r="F16">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.66832597304123131</v>
+      </c>
+      <c r="D17">
+        <v>4.2531287818974652</v>
+      </c>
+      <c r="F17">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.76236412149413024</v>
+      </c>
+      <c r="D2">
+        <v>4.5143492958560814E-2</v>
+      </c>
+      <c r="F2">
+        <v>4393</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.7554648980875629</v>
+      </c>
+      <c r="D3">
+        <v>5.6367574363057497E-2</v>
+      </c>
+      <c r="F3">
+        <v>2891</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.7394239789579059</v>
+      </c>
+      <c r="D4">
+        <v>0.10755859842313549</v>
+      </c>
+      <c r="F4">
+        <v>4483</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.73100889152628012</v>
+      </c>
+      <c r="D5">
+        <v>0.16737025201914787</v>
+      </c>
+      <c r="F5">
+        <v>5085</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.72865484435529948</v>
+      </c>
+      <c r="D6">
+        <v>0.19369797832056473</v>
+      </c>
+      <c r="F6">
+        <v>5039</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.72479380212674605</v>
+      </c>
+      <c r="D7">
+        <v>0.25429851828379091</v>
+      </c>
+      <c r="F7">
+        <v>5815</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.72033268759984392</v>
+      </c>
+      <c r="D8">
+        <v>0.39477647949025652</v>
+      </c>
+      <c r="F8">
+        <v>7232</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.71744957380214769</v>
+      </c>
+      <c r="D9">
+        <v>0.60478867615297283</v>
+      </c>
+      <c r="F9">
+        <v>9514</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.71631269096353967</v>
+      </c>
+      <c r="D10">
+        <v>0.73263032495683145</v>
+      </c>
+      <c r="F10">
+        <v>9087</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.71070963720796287</v>
+      </c>
+      <c r="D11">
+        <v>1.6427186744502029</v>
+      </c>
+      <c r="F11">
+        <v>17167</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.70629601336924641</v>
+      </c>
+      <c r="D12">
+        <v>3.0464830908566358</v>
+      </c>
+      <c r="F12">
+        <v>26086</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.70371490551913218</v>
+      </c>
+      <c r="D13">
+        <v>4.8894209673976885</v>
+      </c>
+      <c r="F13">
+        <v>23405</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.70302972609143854</v>
+      </c>
+      <c r="D14">
+        <v>5.6556766869262125</v>
+      </c>
+      <c r="F14">
+        <v>14072</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.70174377553738965</v>
+      </c>
+      <c r="D15">
+        <v>7.6859424122868889</v>
+      </c>
+      <c r="F15">
+        <v>20493</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.69742910397805169</v>
+      </c>
+      <c r="D16">
+        <v>14.561462732684472</v>
+      </c>
+      <c r="F16">
+        <v>57741</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.69682813352657724</v>
+      </c>
+      <c r="D17">
+        <v>18.613458482198251</v>
+      </c>
+      <c r="F17">
+        <v>42328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.76186991482325828</v>
+      </c>
+      <c r="D2">
+        <v>4.6724324378102804E-2</v>
+      </c>
+      <c r="F2">
+        <v>3716</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.75840147377786138</v>
+      </c>
+      <c r="D3">
+        <v>5.2188062621261376E-2</v>
+      </c>
+      <c r="F3">
+        <v>2158</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.75385603144806879</v>
+      </c>
+      <c r="D4">
+        <v>6.6672440464272564E-2</v>
+      </c>
+      <c r="F4">
+        <v>3171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.74975576053793935</v>
+      </c>
+      <c r="D5">
+        <v>9.7463878043194369E-2</v>
+      </c>
+      <c r="F5">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.7476099466023155</v>
+      </c>
+      <c r="D6">
+        <v>0.12158281794445765</v>
+      </c>
+      <c r="F6">
+        <v>4457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.74312091732082308</v>
+      </c>
+      <c r="D7">
+        <v>0.19249059253048034</v>
+      </c>
+      <c r="F7">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.73787402386834511</v>
+      </c>
+      <c r="D8">
+        <v>0.35670172719321774</v>
+      </c>
+      <c r="F8">
+        <v>6016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.72383373318051047</v>
+      </c>
+      <c r="D9">
+        <v>1.0789618866121891</v>
+      </c>
+      <c r="F9">
+        <v>16469</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.7228838550284411</v>
+      </c>
+      <c r="D10">
+        <v>1.1850672870595931</v>
+      </c>
+      <c r="F10">
+        <v>11322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.72127181117087191</v>
+      </c>
+      <c r="D11">
+        <v>1.4396618030239434</v>
+      </c>
+      <c r="F11">
+        <v>13198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.71887572689706525</v>
+      </c>
+      <c r="D12">
+        <v>2.2096319701593607</v>
+      </c>
+      <c r="F12">
+        <v>26255</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.71735874563517676</v>
+      </c>
+      <c r="D13">
+        <v>3.2950681077748047</v>
+      </c>
+      <c r="F13">
+        <v>35569</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.71692326980985444</v>
+      </c>
+      <c r="D14">
+        <v>3.7825142186560776</v>
+      </c>
+      <c r="F14">
+        <v>22288</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.71612078067264107</v>
+      </c>
+      <c r="D15">
+        <v>5.0563139489368298</v>
+      </c>
+      <c r="F15">
+        <v>23483</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.7150778829294806</v>
+      </c>
+      <c r="D16">
+        <v>8.2335963939262111</v>
+      </c>
+      <c r="F16">
+        <v>37057</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.71475476782735314</v>
+      </c>
+      <c r="D17">
+        <v>10.363926401084274</v>
+      </c>
+      <c r="F17">
+        <v>36622</v>
       </c>
     </row>
   </sheetData>
@@ -2838,6 +4394,190 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.77716455328614087</v>
+      </c>
+      <c r="D2">
+        <v>4.8789511002059943E-2</v>
+      </c>
+      <c r="F2">
+        <v>3104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.77333702775012425</v>
+      </c>
+      <c r="D3">
+        <v>5.481689957026703E-2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
@@ -4205,7 +5945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
combined Nika and Nick's workbooks
</commit_message>
<xml_diff>
--- a/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
+++ b/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvafadar\Desktop\L-curve_Summer2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\Lab Records\L-curve_Analysis_Summer-2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="9015" firstSheet="16" activeTab="19"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="9015" tabRatio="851"/>
   </bookViews>
   <sheets>
     <sheet name="key-to-input-workbooks" sheetId="2" r:id="rId1"/>
@@ -32,6 +32,25 @@
     <sheet name="L-curve_17" sheetId="20" r:id="rId18"/>
     <sheet name="L-curve_18" sheetId="21" r:id="rId19"/>
     <sheet name="L-curve_19" sheetId="22" r:id="rId20"/>
+    <sheet name="L-curve_20" sheetId="23" r:id="rId21"/>
+    <sheet name="L-curve_21" sheetId="24" r:id="rId22"/>
+    <sheet name="L-curve_22" sheetId="25" r:id="rId23"/>
+    <sheet name="L-curve_23" sheetId="26" r:id="rId24"/>
+    <sheet name="L-curve_24" sheetId="27" r:id="rId25"/>
+    <sheet name="L-curve_25" sheetId="28" r:id="rId26"/>
+    <sheet name="L-curve_26" sheetId="29" r:id="rId27"/>
+    <sheet name="L-curve_27" sheetId="30" r:id="rId28"/>
+    <sheet name="L-curve_28" sheetId="31" r:id="rId29"/>
+    <sheet name="L-curve_29" sheetId="32" r:id="rId30"/>
+    <sheet name="L-curve_30" sheetId="33" r:id="rId31"/>
+    <sheet name="L-curve_31" sheetId="34" r:id="rId32"/>
+    <sheet name="L-curve_32" sheetId="35" r:id="rId33"/>
+    <sheet name="L-curve_33" sheetId="36" r:id="rId34"/>
+    <sheet name="L-curve_34" sheetId="41" r:id="rId35"/>
+    <sheet name="L-curve_35" sheetId="42" r:id="rId36"/>
+    <sheet name="L-curve_36" sheetId="43" r:id="rId37"/>
+    <sheet name="L-curve_37" sheetId="44" r:id="rId38"/>
+    <sheet name="L-curve_38" sheetId="45" r:id="rId39"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -43,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="48">
   <si>
     <t>Alpha</t>
   </si>
@@ -193,8 +212,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -221,18 +242,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -247,14 +262,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,20 +553,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="134.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="134.28515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>31</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -558,7 +572,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -566,7 +580,7 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -574,7 +588,7 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -598,7 +612,7 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -606,7 +620,7 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -614,7 +628,7 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -622,7 +636,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="4" t="s">
         <v>22</v>
       </c>
     </row>
@@ -630,7 +644,7 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
     </row>
@@ -638,7 +652,7 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>24</v>
       </c>
     </row>
@@ -646,7 +660,7 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="4" t="s">
         <v>25</v>
       </c>
     </row>
@@ -654,7 +668,7 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -670,7 +684,7 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
     </row>
@@ -678,7 +692,7 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="4" t="s">
         <v>12</v>
       </c>
     </row>
@@ -686,7 +700,7 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="4" t="s">
         <v>11</v>
       </c>
     </row>
@@ -694,7 +708,7 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="4" t="s">
         <v>10</v>
       </c>
     </row>
@@ -702,7 +716,7 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
     </row>
@@ -710,7 +724,7 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -718,7 +732,7 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -726,7 +740,7 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -734,7 +748,7 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>5</v>
       </c>
     </row>
@@ -742,7 +756,7 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
     </row>
@@ -750,7 +764,7 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -758,7 +772,7 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -766,7 +780,7 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
     </row>
@@ -774,7 +788,7 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -782,7 +796,7 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -790,7 +804,7 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -798,7 +812,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -806,7 +820,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>27</v>
       </c>
     </row>
@@ -814,7 +828,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -822,7 +836,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="4" t="s">
         <v>29</v>
       </c>
     </row>
@@ -830,7 +844,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="4" t="s">
         <v>15</v>
       </c>
     </row>
@@ -838,7 +852,7 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -846,7 +860,7 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -854,7 +868,7 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -4398,7 +4412,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -4574,6 +4588,1900 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.79561300000000001</v>
+      </c>
+      <c r="D2" s="5">
+        <v>5.5077000000000001E-2</v>
+      </c>
+      <c r="F2">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.79169599999999996</v>
+      </c>
+      <c r="D3" s="5">
+        <v>6.1234999999999998E-2</v>
+      </c>
+      <c r="F3">
+        <v>1519</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.78730199999999995</v>
+      </c>
+      <c r="D4" s="5">
+        <v>7.4854000000000004E-2</v>
+      </c>
+      <c r="F4">
+        <v>1925</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.78516600000000003</v>
+      </c>
+      <c r="D5" s="5">
+        <v>9.0206999999999996E-2</v>
+      </c>
+      <c r="F5">
+        <v>2678</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.78442299999999998</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9.8545999999999995E-2</v>
+      </c>
+      <c r="F6">
+        <v>2416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.78250299999999995</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.12948899999999999</v>
+      </c>
+      <c r="F7">
+        <v>3027</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.77431899999999998</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.44880300000000001</v>
+      </c>
+      <c r="F8">
+        <v>5498</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.76992499999999997</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.74981399999999998</v>
+      </c>
+      <c r="F9">
+        <v>5177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.76908500000000002</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.84362599999999999</v>
+      </c>
+      <c r="F10">
+        <v>5563</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.76771400000000001</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.05983</v>
+      </c>
+      <c r="F11">
+        <v>5328</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.76592300000000002</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.624252</v>
+      </c>
+      <c r="F12">
+        <v>10808</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.76505800000000002</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2.234686</v>
+      </c>
+      <c r="F13">
+        <v>17626</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.764845</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2.4730300000000001</v>
+      </c>
+      <c r="F14">
+        <v>20512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.76447500000000002</v>
+      </c>
+      <c r="D15">
+        <v>3.0567959999999998</v>
+      </c>
+      <c r="F15">
+        <v>18748</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.76375499999999996</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5.523002</v>
+      </c>
+      <c r="F16">
+        <v>31172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.76284099999999999</v>
+      </c>
+      <c r="D17" s="6">
+        <v>11.812939999999999</v>
+      </c>
+      <c r="F17">
+        <v>37328</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.82028299999999998</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3.9623999999999999E-2</v>
+      </c>
+      <c r="F2">
+        <v>1905</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.81631299999999996</v>
+      </c>
+      <c r="D3">
+        <v>4.5878000000000002E-2</v>
+      </c>
+      <c r="F3">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.81157299999999999</v>
+      </c>
+      <c r="D4">
+        <v>6.0649000000000002E-2</v>
+      </c>
+      <c r="F4">
+        <v>1333</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.80917600000000001</v>
+      </c>
+      <c r="D5">
+        <v>7.7882000000000007E-2</v>
+      </c>
+      <c r="F5">
+        <v>1884</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.808342</v>
+      </c>
+      <c r="D6">
+        <v>8.7243000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.80617099999999997</v>
+      </c>
+      <c r="D7">
+        <v>0.12224400000000001</v>
+      </c>
+      <c r="F7">
+        <v>2314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.80229600000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.24330299999999999</v>
+      </c>
+      <c r="F8">
+        <v>2914</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.79327800000000004</v>
+      </c>
+      <c r="D9">
+        <v>0.78342500000000004</v>
+      </c>
+      <c r="F9">
+        <v>5011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.79240299999999997</v>
+      </c>
+      <c r="D10">
+        <v>0.88105599999999995</v>
+      </c>
+      <c r="F10">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.79096</v>
+      </c>
+      <c r="D11">
+        <v>1.108789</v>
+      </c>
+      <c r="F11">
+        <v>5555</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.78894600000000004</v>
+      </c>
+      <c r="D12">
+        <v>1.748054</v>
+      </c>
+      <c r="F12">
+        <v>7429</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.787856</v>
+      </c>
+      <c r="D13">
+        <v>2.5180530000000001</v>
+      </c>
+      <c r="F13">
+        <v>14557</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.787578</v>
+      </c>
+      <c r="D14">
+        <v>2.8278479999999999</v>
+      </c>
+      <c r="F14">
+        <v>10686</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.78709799999999996</v>
+      </c>
+      <c r="D15">
+        <v>3.5887880000000001</v>
+      </c>
+      <c r="F15">
+        <v>10422</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.78641499999999998</v>
+      </c>
+      <c r="D16">
+        <v>5.7745259999999998</v>
+      </c>
+      <c r="F16">
+        <v>18630</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.78570700000000004</v>
+      </c>
+      <c r="D17">
+        <v>11.012869999999999</v>
+      </c>
+      <c r="F17">
+        <v>23698</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.911049</v>
+      </c>
+      <c r="D2" s="5">
+        <v>4.3668999999999999E-2</v>
+      </c>
+      <c r="F2">
+        <v>1309</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.90627100000000005</v>
+      </c>
+      <c r="D3" s="5">
+        <v>5.1194999999999997E-2</v>
+      </c>
+      <c r="F3">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.90058899999999997</v>
+      </c>
+      <c r="D4" s="5">
+        <v>6.8884000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.89776100000000003</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8.9200000000000002E-2</v>
+      </c>
+      <c r="F5">
+        <v>1412</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.89678100000000005</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.10020800000000001</v>
+      </c>
+      <c r="F6">
+        <v>1471</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.894208</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.14171600000000001</v>
+      </c>
+      <c r="F7">
+        <v>1591</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.88959600000000005</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.28540500000000002</v>
+      </c>
+      <c r="F8">
+        <v>2173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.880907</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.85133700000000001</v>
+      </c>
+      <c r="F9">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.87997700000000001</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.95500300000000005</v>
+      </c>
+      <c r="F10">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.87862799999999996</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.1664129999999999</v>
+      </c>
+      <c r="F11">
+        <v>3138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.87717800000000001</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1.6180289999999999</v>
+      </c>
+      <c r="F12">
+        <v>5578</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.87649299999999997</v>
+      </c>
+      <c r="D13" s="5">
+        <v>2.1055649999999999</v>
+      </c>
+      <c r="F13">
+        <v>6288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.87629299999999999</v>
+      </c>
+      <c r="D14" s="5">
+        <v>2.32999</v>
+      </c>
+      <c r="F14">
+        <v>5327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.87584499999999998</v>
+      </c>
+      <c r="D15" s="5">
+        <v>3.0476429999999999</v>
+      </c>
+      <c r="F15">
+        <v>10071</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.87428099999999997</v>
+      </c>
+      <c r="D16" s="5">
+        <v>8.5875529999999998</v>
+      </c>
+      <c r="F16">
+        <v>19707</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.87256900000000004</v>
+      </c>
+      <c r="D17" s="6">
+        <v>20.343769999999999</v>
+      </c>
+      <c r="F17">
+        <v>8795</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.90961400000000003</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3.8592000000000001E-2</v>
+      </c>
+      <c r="F2">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.90677799999999997</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4.3091999999999998E-2</v>
+      </c>
+      <c r="F3">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.90237800000000001</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5.7159000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.89959900000000004</v>
+      </c>
+      <c r="D5" s="5">
+        <v>7.7237E-2</v>
+      </c>
+      <c r="F5">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.89859</v>
+      </c>
+      <c r="D6" s="5">
+        <v>8.8568999999999995E-2</v>
+      </c>
+      <c r="F6">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.895845</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.13295799999999999</v>
+      </c>
+      <c r="F7">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.890957</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.28337099999999998</v>
+      </c>
+      <c r="F8">
+        <v>1435</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.88931400000000005</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.39913799999999999</v>
+      </c>
+      <c r="F9">
+        <v>2299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.88802400000000004</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.54540100000000002</v>
+      </c>
+      <c r="F10">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.88351299999999999</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.2791090000000001</v>
+      </c>
+      <c r="F11">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.872784</v>
+      </c>
+      <c r="D12" s="5">
+        <v>4.6713560000000003</v>
+      </c>
+      <c r="F12">
+        <v>2341</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.86825300000000005</v>
+      </c>
+      <c r="D13" s="5">
+        <v>7.8478659999999998</v>
+      </c>
+      <c r="F13">
+        <v>2084</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.86721000000000004</v>
+      </c>
+      <c r="D14" s="5">
+        <v>9.0115739999999995</v>
+      </c>
+      <c r="F14">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.86549500000000001</v>
+      </c>
+      <c r="D15" s="6">
+        <v>11.690099999999999</v>
+      </c>
+      <c r="F15">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.86465499999999995</v>
+      </c>
+      <c r="D16" s="6">
+        <v>14.07443</v>
+      </c>
+      <c r="F16">
+        <v>1738</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.86465499999999995</v>
+      </c>
+      <c r="D17" s="6">
+        <v>14.07443</v>
+      </c>
+      <c r="F17">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1.088158</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3.4117000000000001E-2</v>
+      </c>
+      <c r="F2">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1.0852059999999999</v>
+      </c>
+      <c r="D3" s="5">
+        <v>3.8807000000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>1.080344</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5.4455000000000003E-2</v>
+      </c>
+      <c r="F4">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.077102</v>
+      </c>
+      <c r="D5" s="5">
+        <v>7.7882999999999994E-2</v>
+      </c>
+      <c r="F5">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1.0759479999999999</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9.0838000000000002E-2</v>
+      </c>
+      <c r="F6">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1.072803</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.14181099999999999</v>
+      </c>
+      <c r="F7">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1.0654600000000001</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.37390699999999999</v>
+      </c>
+      <c r="F8">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1.0628200000000001</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.55657500000000004</v>
+      </c>
+      <c r="F9">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1.062276</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.61726199999999998</v>
+      </c>
+      <c r="F10">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1.0613539999999999</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.763104</v>
+      </c>
+      <c r="F11">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1.0566770000000001</v>
+      </c>
+      <c r="D12" s="5">
+        <v>2.3751340000000001</v>
+      </c>
+      <c r="F12">
+        <v>1159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1.054835</v>
+      </c>
+      <c r="D13" s="5">
+        <v>3.6678039999999998</v>
+      </c>
+      <c r="F13">
+        <v>849</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1.0543990000000001</v>
+      </c>
+      <c r="D14" s="5">
+        <v>4.1556030000000002</v>
+      </c>
+      <c r="F14">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1.0536570000000001</v>
+      </c>
+      <c r="D15" s="5">
+        <v>5.3260310000000004</v>
+      </c>
+      <c r="F15">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>1.052713</v>
+      </c>
+      <c r="D16" s="5">
+        <v>8.2841609999999992</v>
+      </c>
+      <c r="F16">
+        <v>898</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>1.0522830000000001</v>
+      </c>
+      <c r="D17" s="6">
+        <v>11.304959999999999</v>
+      </c>
+      <c r="F17">
+        <v>849</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.781362</v>
+      </c>
+      <c r="D2" s="5">
+        <v>3.7957999999999999E-2</v>
+      </c>
+      <c r="F2">
+        <v>5821</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.78020599999999996</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4.2890999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>6048</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.77824000000000004</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5.0349999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>5482</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.77367399999999997</v>
+      </c>
+      <c r="D5" s="5">
+        <v>8.4301000000000001E-2</v>
+      </c>
+      <c r="F5">
+        <v>6905</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0.77238300000000004</v>
+      </c>
+      <c r="D6" s="5">
+        <v>9.8834000000000005E-2</v>
+      </c>
+      <c r="F6">
+        <v>6337</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.76934899999999995</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.14769599999999999</v>
+      </c>
+      <c r="F7">
+        <v>8560</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.76215699999999997</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.39043600000000001</v>
+      </c>
+      <c r="F8">
+        <v>14207</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.75368100000000005</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.99561699999999997</v>
+      </c>
+      <c r="F9">
+        <v>21972</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.75137500000000002</v>
+      </c>
+      <c r="D10" s="5">
+        <v>1.2532840000000001</v>
+      </c>
+      <c r="F10">
+        <v>21466</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0.747888</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1.8012010000000001</v>
+      </c>
+      <c r="F11">
+        <v>23641</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.743085</v>
+      </c>
+      <c r="D12" s="5">
+        <v>3.3332199999999998</v>
+      </c>
+      <c r="F12">
+        <v>43862</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.73970100000000005</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5.3484660000000002</v>
+      </c>
+      <c r="F13">
+        <v>110189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14" s="5">
+        <v>0.73909899999999995</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5.9845329999999999</v>
+      </c>
+      <c r="F14">
+        <v>81983</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15" s="5">
+        <v>0.73851999999999995</v>
+      </c>
+      <c r="D15" s="5">
+        <v>6.8936580000000003</v>
+      </c>
+      <c r="F15">
+        <v>75037</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.73851999999999995</v>
+      </c>
+      <c r="D16" s="5">
+        <v>6.8936279999999996</v>
+      </c>
+      <c r="F16">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.73743099999999995</v>
+      </c>
+      <c r="D17" s="6">
+        <v>11.874309999999999</v>
+      </c>
+      <c r="F17">
+        <v>83852</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4896,6 +6804,128 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S34" sqref="S34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H17"/>

</xml_diff>

<commit_message>
final compiled L-curve data
runs 1 through 38
</commit_message>
<xml_diff>
--- a/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
+++ b/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kdahlqui\Documents\Lab Records\L-curve_Analysis_Summer-2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nvafadar\Desktop\L-curve_Summer2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="9015" tabRatio="851" firstSheet="17" activeTab="20"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19215" windowHeight="9015" tabRatio="851" firstSheet="33" activeTab="39"/>
   </bookViews>
   <sheets>
     <sheet name="key-to-input-workbooks" sheetId="2" r:id="rId1"/>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="55">
   <si>
     <t>Alpha</t>
   </si>
@@ -575,8 +575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -836,7 +836,7 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="7" t="s">
         <v>37</v>
       </c>
     </row>
@@ -844,7 +844,7 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="7" t="s">
         <v>27</v>
       </c>
     </row>
@@ -852,7 +852,7 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="4" t="s">
+      <c r="B34" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -860,7 +860,7 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="7" t="s">
         <v>29</v>
       </c>
     </row>
@@ -868,7 +868,7 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="7" t="s">
         <v>15</v>
       </c>
     </row>
@@ -5318,7 +5318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6867,7 +6867,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G17"/>
+      <selection activeCell="C1" sqref="C1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7174,24 +7174,620 @@
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.78025740711169977</v>
+      </c>
+      <c r="D2">
+        <v>3.7973821073067293E-2</v>
+      </c>
+      <c r="F2">
+        <v>5863</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.77911596222471702</v>
+      </c>
+      <c r="D3">
+        <v>4.1491232488790913E-2</v>
+      </c>
+      <c r="F3">
+        <v>6211</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.77728483125697223</v>
+      </c>
+      <c r="D4">
+        <v>4.804215745165441E-2</v>
+      </c>
+      <c r="F4">
+        <v>5520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.75969059645324211</v>
+      </c>
+      <c r="D5">
+        <v>0.18828001358417615</v>
+      </c>
+      <c r="F5">
+        <v>12021</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.75500781343546275</v>
+      </c>
+      <c r="D6">
+        <v>0.24112932120613892</v>
+      </c>
+      <c r="F6">
+        <v>10278</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.72405599074368343</v>
+      </c>
+      <c r="D7">
+        <v>0.69065262197759902</v>
+      </c>
+      <c r="F7">
+        <v>14454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.70342334997328892</v>
+      </c>
+      <c r="D8">
+        <v>1.3175727732862521</v>
+      </c>
+      <c r="F8">
+        <v>13642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.69516900771528445</v>
+      </c>
+      <c r="D9">
+        <v>1.8987962118469592</v>
+      </c>
+      <c r="F9">
+        <v>17949</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.69321999910461329</v>
+      </c>
+      <c r="D10">
+        <v>2.116501495190676</v>
+      </c>
+      <c r="F10">
+        <v>25912</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.69004966336733209</v>
+      </c>
+      <c r="D11">
+        <v>2.6152208700914086</v>
+      </c>
+      <c r="F11">
+        <v>27835</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.68642957418677764</v>
+      </c>
+      <c r="D12">
+        <v>3.7441669778942646</v>
+      </c>
+      <c r="F12">
+        <v>49877</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.68346626532839694</v>
+      </c>
+      <c r="D13">
+        <v>4.9236867689169417</v>
+      </c>
+      <c r="F13">
+        <v>103820</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.68301430269224872</v>
+      </c>
+      <c r="D14">
+        <v>5.4293677579650099</v>
+      </c>
+      <c r="F14">
+        <v>58624</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.68221241656690357</v>
+      </c>
+      <c r="D15">
+        <v>6.694976616612391</v>
+      </c>
+      <c r="F15">
+        <v>172473</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.67949564040507549</v>
+      </c>
+      <c r="D16">
+        <v>15.101368621688035</v>
+      </c>
+      <c r="F16">
+        <v>136232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.67949576352277741</v>
+      </c>
+      <c r="D17">
+        <v>15.101371772280896</v>
+      </c>
+      <c r="F17">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.76600065444362109</v>
+      </c>
+      <c r="D2">
+        <v>4.8074049909900156E-2</v>
+      </c>
+      <c r="F2">
+        <v>5876</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.76044026605227188</v>
+      </c>
+      <c r="D3">
+        <v>6.7479067358409084E-2</v>
+      </c>
+      <c r="F3">
+        <v>6218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.75290624421317209</v>
+      </c>
+      <c r="D4">
+        <v>9.8800905096309039E-2</v>
+      </c>
+      <c r="F4">
+        <v>4797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.7465857002714501</v>
+      </c>
+      <c r="D5">
+        <v>0.1525399353846594</v>
+      </c>
+      <c r="F5">
+        <v>8386</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.74312201550053669</v>
+      </c>
+      <c r="D6">
+        <v>0.19591457628276401</v>
+      </c>
+      <c r="F6">
+        <v>9585</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.72569817227343469</v>
+      </c>
+      <c r="D7">
+        <v>0.45618258326811401</v>
+      </c>
+      <c r="F7">
+        <v>14775</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.70847992970654539</v>
+      </c>
+      <c r="D8">
+        <v>1.0143097602712026</v>
+      </c>
+      <c r="F8">
+        <v>20906</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.70371962080507477</v>
+      </c>
+      <c r="D9">
+        <v>1.3532770163741294</v>
+      </c>
+      <c r="F9">
+        <v>30052</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.70264027481911973</v>
+      </c>
+      <c r="D10">
+        <v>1.4764614749146274</v>
+      </c>
+      <c r="F10">
+        <v>37845</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.70106089631948221</v>
+      </c>
+      <c r="D11">
+        <v>1.7263057075362644</v>
+      </c>
+      <c r="F11">
+        <v>44716</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.6994049356405424</v>
+      </c>
+      <c r="D12">
+        <v>2.2426739682317769</v>
+      </c>
+      <c r="F12">
+        <v>66935</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.69827196023983917</v>
+      </c>
+      <c r="D13">
+        <v>3.2041162406449346</v>
+      </c>
+      <c r="F13">
+        <v>73179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.69790802008541974</v>
+      </c>
+      <c r="D14">
+        <v>3.6651944702448094</v>
+      </c>
+      <c r="F14">
+        <v>40867</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.69725999856944476</v>
+      </c>
+      <c r="D15">
+        <v>4.6546304696757757</v>
+      </c>
+      <c r="F15">
+        <v>35933</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.69682112183408118</v>
+      </c>
+      <c r="D16">
+        <v>6.3246552239573148</v>
+      </c>
+      <c r="F16">
+        <v>34727</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.696268469857526</v>
+      </c>
+      <c r="D17">
+        <v>9.7283433308987775</v>
+      </c>
+      <c r="F17">
+        <v>126013</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7200,7 +7796,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -7936,120 +8534,3101 @@
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.75781639699153647</v>
+      </c>
+      <c r="D2">
+        <v>5.0124478807429533E-2</v>
+      </c>
+      <c r="F2">
+        <v>6163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.74971654095517226</v>
+      </c>
+      <c r="D3">
+        <v>6.8340599507419983E-2</v>
+      </c>
+      <c r="F3">
+        <v>6562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.73796419387585466</v>
+      </c>
+      <c r="D4">
+        <v>0.1082244106448059</v>
+      </c>
+      <c r="F4">
+        <v>5883</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.729702254849107</v>
+      </c>
+      <c r="D5">
+        <v>0.16644639954830848</v>
+      </c>
+      <c r="F5">
+        <v>7307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.72798920182335203</v>
+      </c>
+      <c r="D6">
+        <v>0.18575075200375918</v>
+      </c>
+      <c r="F6">
+        <v>7020</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.72441223854038916</v>
+      </c>
+      <c r="D7">
+        <v>0.24310056746692751</v>
+      </c>
+      <c r="F7">
+        <v>8616</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.71398668251381892</v>
+      </c>
+      <c r="D8">
+        <v>0.59317792843156314</v>
+      </c>
+      <c r="F8">
+        <v>13919</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.7077828096636668</v>
+      </c>
+      <c r="D9">
+        <v>1.0241447099141721</v>
+      </c>
+      <c r="F9">
+        <v>21290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.70648887640327329</v>
+      </c>
+      <c r="D10">
+        <v>1.1686231175210706</v>
+      </c>
+      <c r="F10">
+        <v>20094</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.7044056424174453</v>
+      </c>
+      <c r="D11">
+        <v>1.4962874019277856</v>
+      </c>
+      <c r="F11">
+        <v>24998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.70163645248395123</v>
+      </c>
+      <c r="D12">
+        <v>2.3833570345621098</v>
+      </c>
+      <c r="F12">
+        <v>70999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.6997949107563276</v>
+      </c>
+      <c r="D13">
+        <v>3.4913925604129434</v>
+      </c>
+      <c r="F13">
+        <v>141735</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.69947513753842927</v>
+      </c>
+      <c r="D14">
+        <v>3.8515110740212957</v>
+      </c>
+      <c r="F14">
+        <v>69545</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.69887607563993104</v>
+      </c>
+      <c r="D15">
+        <v>4.8103089872301226</v>
+      </c>
+      <c r="F15">
+        <v>137626</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.69725461420968449</v>
+      </c>
+      <c r="D16">
+        <v>9.3106883732041119</v>
+      </c>
+      <c r="F16">
+        <v>61889</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.69743579941137801</v>
+      </c>
+      <c r="D17">
+        <v>11.880012814976126</v>
+      </c>
+      <c r="F17">
+        <v>103044</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.78290619605808043</v>
+      </c>
+      <c r="D2">
+        <v>4.1623762857562294E-2</v>
+      </c>
+      <c r="F2">
+        <v>5395</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.78538358758872417</v>
+      </c>
+      <c r="D3">
+        <v>9.6268802172443588E-2</v>
+      </c>
+      <c r="F3">
+        <v>5011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.78534991117943187</v>
+      </c>
+      <c r="D4">
+        <v>0.21729487779579484</v>
+      </c>
+      <c r="F4">
+        <v>7927</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.80272935767028408</v>
+      </c>
+      <c r="D5">
+        <v>0.75454326017306084</v>
+      </c>
+      <c r="F5">
+        <v>10018</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>1.7712027747360073</v>
+      </c>
+      <c r="D6">
+        <v>2.4822174588293673</v>
+      </c>
+      <c r="F6">
+        <v>12054</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>6.8827510643749275</v>
+      </c>
+      <c r="D7">
+        <v>3.9398736465279738</v>
+      </c>
+      <c r="F7">
+        <v>13166</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>6.867138348530009</v>
+      </c>
+      <c r="D8">
+        <v>4.4680238592285386</v>
+      </c>
+      <c r="F8">
+        <v>21414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>6.8586643122156845</v>
+      </c>
+      <c r="D9">
+        <v>5.0402187285304096</v>
+      </c>
+      <c r="F9">
+        <v>17576</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>6.8572165127494493</v>
+      </c>
+      <c r="D10">
+        <v>5.2017469212508232</v>
+      </c>
+      <c r="F10">
+        <v>22899</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>6.8550084547518129</v>
+      </c>
+      <c r="D11">
+        <v>5.5583405012460503</v>
+      </c>
+      <c r="F11">
+        <v>36586</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>6.8504637718519401</v>
+      </c>
+      <c r="D12">
+        <v>6.9763816762729602</v>
+      </c>
+      <c r="F12">
+        <v>54136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>6.8484812862087665</v>
+      </c>
+      <c r="D13">
+        <v>8.5923340677439377</v>
+      </c>
+      <c r="F13">
+        <v>57043</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>6.8485611164536628</v>
+      </c>
+      <c r="D14">
+        <v>8.592389100272058</v>
+      </c>
+      <c r="F14">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>6.8474022110704951</v>
+      </c>
+      <c r="D15">
+        <v>10.213098194964244</v>
+      </c>
+      <c r="F15">
+        <v>66276</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>6.849899051194261</v>
+      </c>
+      <c r="D16">
+        <v>12.044231837766791</v>
+      </c>
+      <c r="F16">
+        <v>20164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>6.8394601079020516</v>
+      </c>
+      <c r="D17">
+        <v>15.317516286295247</v>
+      </c>
+      <c r="F17">
+        <v>27035</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.77185048678360713</v>
+      </c>
+      <c r="D2">
+        <v>3.9420841856249327E-2</v>
+      </c>
+      <c r="F2">
+        <v>6037</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.76935048971206355</v>
+      </c>
+      <c r="D3">
+        <v>4.7485026222406676E-2</v>
+      </c>
+      <c r="F3">
+        <v>6791</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.76411055365920588</v>
+      </c>
+      <c r="D4">
+        <v>6.7347044332132872E-2</v>
+      </c>
+      <c r="F4">
+        <v>6621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.74621049394416428</v>
+      </c>
+      <c r="D5">
+        <v>0.20697258229790771</v>
+      </c>
+      <c r="F5">
+        <v>10274</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.74060109693956189</v>
+      </c>
+      <c r="D6">
+        <v>0.26984819518370168</v>
+      </c>
+      <c r="F6">
+        <v>7778</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.73016299035142629</v>
+      </c>
+      <c r="D7">
+        <v>0.43844889637166973</v>
+      </c>
+      <c r="F7">
+        <v>11027</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.70966445652766219</v>
+      </c>
+      <c r="D8">
+        <v>1.0337593163152408</v>
+      </c>
+      <c r="F8">
+        <v>15321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.70472921785344267</v>
+      </c>
+      <c r="D9">
+        <v>1.3741581281627744</v>
+      </c>
+      <c r="F9">
+        <v>17713</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.70372998294630595</v>
+      </c>
+      <c r="D10">
+        <v>1.485717199446015</v>
+      </c>
+      <c r="F10">
+        <v>9647</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.70173402010944108</v>
+      </c>
+      <c r="D11">
+        <v>1.7965656875819989</v>
+      </c>
+      <c r="F11">
+        <v>32637</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.69964620930045374</v>
+      </c>
+      <c r="D12">
+        <v>2.4703801554411413</v>
+      </c>
+      <c r="F12">
+        <v>50912</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.69680128350074066</v>
+      </c>
+      <c r="D13">
+        <v>3.8816174234374281</v>
+      </c>
+      <c r="F13">
+        <v>22824</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.69910552312462459</v>
+      </c>
+      <c r="D14">
+        <v>6.1934992512405191</v>
+      </c>
+      <c r="F14">
+        <v>38659</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.69773139976888088</v>
+      </c>
+      <c r="D15">
+        <v>6.1811751111607238</v>
+      </c>
+      <c r="F15">
+        <v>41349</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.6977314026952105</v>
+      </c>
+      <c r="D16">
+        <v>6.1811773037533984</v>
+      </c>
+      <c r="F16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.6977314026952105</v>
+      </c>
+      <c r="D17">
+        <v>6.1811773037533984</v>
+      </c>
+      <c r="F17">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.76350028516889212</v>
+      </c>
+      <c r="D2">
+        <v>4.6184276950771513E-2</v>
+      </c>
+      <c r="F2">
+        <v>6040</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.75749993180800912</v>
+      </c>
+      <c r="D3">
+        <v>5.7624735196097031E-2</v>
+      </c>
+      <c r="F3">
+        <v>6444</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.74516898853991376</v>
+      </c>
+      <c r="D4">
+        <v>0.10205803973172017</v>
+      </c>
+      <c r="F4">
+        <v>6331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.73650107580314217</v>
+      </c>
+      <c r="D5">
+        <v>0.16230070100695596</v>
+      </c>
+      <c r="F5">
+        <v>7372</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.73461358745440675</v>
+      </c>
+      <c r="D6">
+        <v>0.18344173557934904</v>
+      </c>
+      <c r="F6">
+        <v>7604</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.73108702052622676</v>
+      </c>
+      <c r="D7">
+        <v>0.23951764842410317</v>
+      </c>
+      <c r="F7">
+        <v>10505</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.71302947870519429</v>
+      </c>
+      <c r="D8">
+        <v>0.69433465735643385</v>
+      </c>
+      <c r="F8">
+        <v>17582</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.70887241667058876</v>
+      </c>
+      <c r="D9">
+        <v>0.99589019267638568</v>
+      </c>
+      <c r="F9">
+        <v>19853</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.70232218295167759</v>
+      </c>
+      <c r="D10">
+        <v>1.4967659300084959</v>
+      </c>
+      <c r="F10">
+        <v>26245</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.69962404448103499</v>
+      </c>
+      <c r="D11">
+        <v>1.9340486854086671</v>
+      </c>
+      <c r="F11">
+        <v>17822</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.69467500391082981</v>
+      </c>
+      <c r="D12">
+        <v>3.5601092887898913</v>
+      </c>
+      <c r="F12">
+        <v>19681</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.69220718020339111</v>
+      </c>
+      <c r="D13">
+        <v>5.394939297414032</v>
+      </c>
+      <c r="F13">
+        <v>17570</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.69220717758753314</v>
+      </c>
+      <c r="D14">
+        <v>5.3949420177480345</v>
+      </c>
+      <c r="F14">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.69220717821621269</v>
+      </c>
+      <c r="D15">
+        <v>5.3949420730796458</v>
+      </c>
+      <c r="F15">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.69220717821621269</v>
+      </c>
+      <c r="D16">
+        <v>5.3949420730796458</v>
+      </c>
+      <c r="F16">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.69220717821621269</v>
+      </c>
+      <c r="D17">
+        <v>5.3949420730796458</v>
+      </c>
+      <c r="F17">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.76942744794134521</v>
+      </c>
+      <c r="D2">
+        <v>4.2596550015266688E-2</v>
+      </c>
+      <c r="F2">
+        <v>5425</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.76470942983703438</v>
+      </c>
+      <c r="D3">
+        <v>5.5932398047594152E-2</v>
+      </c>
+      <c r="F3">
+        <v>6048</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.75210590485578943</v>
+      </c>
+      <c r="D4">
+        <v>0.10135849340679884</v>
+      </c>
+      <c r="F4">
+        <v>5595</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.74503954352844626</v>
+      </c>
+      <c r="D5">
+        <v>0.15070816827218295</v>
+      </c>
+      <c r="F5">
+        <v>7074</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.74333270834272569</v>
+      </c>
+      <c r="D6">
+        <v>0.17013250136181554</v>
+      </c>
+      <c r="F6">
+        <v>8556</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.70845979723929342</v>
+      </c>
+      <c r="D7">
+        <v>0.70348407330955998</v>
+      </c>
+      <c r="F7">
+        <v>14088</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.69894693190274326</v>
+      </c>
+      <c r="D8">
+        <v>0.99650306567054237</v>
+      </c>
+      <c r="F8">
+        <v>14092</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.69426975242246036</v>
+      </c>
+      <c r="D9">
+        <v>1.3325427753012704</v>
+      </c>
+      <c r="F9">
+        <v>18672</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.69281323530418082</v>
+      </c>
+      <c r="D10">
+        <v>1.4955445954191746</v>
+      </c>
+      <c r="F10">
+        <v>15254</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.68892725342897154</v>
+      </c>
+      <c r="D11">
+        <v>2.0862547094749027</v>
+      </c>
+      <c r="F11">
+        <v>34702</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.68503689011388114</v>
+      </c>
+      <c r="D12">
+        <v>3.4316680293173363</v>
+      </c>
+      <c r="F12">
+        <v>63462</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.6939469860103904</v>
+      </c>
+      <c r="D13">
+        <v>4.1171933255487003</v>
+      </c>
+      <c r="F13">
+        <v>200214</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.69334988057232982</v>
+      </c>
+      <c r="D14">
+        <v>4.787265476964917</v>
+      </c>
+      <c r="F14">
+        <v>111712</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.69244536855430805</v>
+      </c>
+      <c r="D15">
+        <v>6.2202139905370917</v>
+      </c>
+      <c r="F15">
+        <v>55487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.69084478842505381</v>
+      </c>
+      <c r="D16">
+        <v>10.586838920687537</v>
+      </c>
+      <c r="F16">
+        <v>114910</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.69064635390684981</v>
+      </c>
+      <c r="D17">
+        <v>12.146227370423633</v>
+      </c>
+      <c r="F17">
+        <v>72017</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.78128016089996066</v>
+      </c>
+      <c r="D2">
+        <v>3.8063729942409801E-2</v>
+      </c>
+      <c r="F2">
+        <v>7025</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.78039716676420212</v>
+      </c>
+      <c r="D3">
+        <v>4.8386469173600295E-2</v>
+      </c>
+      <c r="F3">
+        <v>6907</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.77914968329204248</v>
+      </c>
+      <c r="D4">
+        <v>5.8709020430874961E-2</v>
+      </c>
+      <c r="F4">
+        <v>4708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.77703790104790216</v>
+      </c>
+      <c r="D5">
+        <v>7.9707519762233336E-2</v>
+      </c>
+      <c r="F5">
+        <v>7782</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.77183478695548768</v>
+      </c>
+      <c r="D6">
+        <v>0.14415572141147812</v>
+      </c>
+      <c r="F6">
+        <v>9870</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.75002486074748675</v>
+      </c>
+      <c r="D7">
+        <v>0.46821119121628951</v>
+      </c>
+      <c r="F7">
+        <v>15852</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.7382028348343711</v>
+      </c>
+      <c r="D8">
+        <v>0.79627434048225243</v>
+      </c>
+      <c r="F8">
+        <v>23839</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.73610749913731244</v>
+      </c>
+      <c r="D9">
+        <v>0.94640302992605574</v>
+      </c>
+      <c r="F9">
+        <v>24971</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.73515360179960321</v>
+      </c>
+      <c r="D10">
+        <v>1.0884109584855026</v>
+      </c>
+      <c r="F10">
+        <v>13490</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.73292999073666976</v>
+      </c>
+      <c r="D11">
+        <v>1.3888893020576896</v>
+      </c>
+      <c r="F11">
+        <v>21946</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.72987611799562224</v>
+      </c>
+      <c r="D12">
+        <v>2.2830633872472657</v>
+      </c>
+      <c r="F12">
+        <v>42183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.72921342612850393</v>
+      </c>
+      <c r="D13">
+        <v>2.8248583975553969</v>
+      </c>
+      <c r="F13">
+        <v>27877</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.72904668858965949</v>
+      </c>
+      <c r="D14">
+        <v>2.9168434595114747</v>
+      </c>
+      <c r="F14">
+        <v>62670</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.72874251250301314</v>
+      </c>
+      <c r="D15">
+        <v>3.4136657062413134</v>
+      </c>
+      <c r="F15">
+        <v>74372</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.72805317560670046</v>
+      </c>
+      <c r="D16">
+        <v>5.8174031398155108</v>
+      </c>
+      <c r="F16">
+        <v>50478</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.72806788215822626</v>
+      </c>
+      <c r="D17">
+        <v>6.9999956521933706</v>
+      </c>
+      <c r="F17">
+        <v>34145</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.85177445549488406</v>
+      </c>
+      <c r="D2">
+        <v>4.0385018795477547E-2</v>
+      </c>
+      <c r="F2">
+        <v>9186</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.846570526695409</v>
+      </c>
+      <c r="D3">
+        <v>4.9130338783842264E-2</v>
+      </c>
+      <c r="F3">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.82831628124190981</v>
+      </c>
+      <c r="D4">
+        <v>0.11100698997373146</v>
+      </c>
+      <c r="F4">
+        <v>7988</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.81761270461959401</v>
+      </c>
+      <c r="D5">
+        <v>0.18562116650874846</v>
+      </c>
+      <c r="F5">
+        <v>11002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.81546598133938564</v>
+      </c>
+      <c r="D6">
+        <v>0.20956300295361491</v>
+      </c>
+      <c r="F6">
+        <v>9597</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.80887764207908486</v>
+      </c>
+      <c r="D7">
+        <v>0.32254473838960873</v>
+      </c>
+      <c r="F7">
+        <v>15564</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.7922440734190842</v>
+      </c>
+      <c r="D8">
+        <v>0.64392847285032928</v>
+      </c>
+      <c r="F8">
+        <v>22474</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.78902915506481242</v>
+      </c>
+      <c r="D9">
+        <v>0.87159539604723102</v>
+      </c>
+      <c r="F9">
+        <v>34759</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.78820792036531562</v>
+      </c>
+      <c r="D10">
+        <v>0.96487185746746418</v>
+      </c>
+      <c r="F10">
+        <v>30190</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.78672268197359363</v>
+      </c>
+      <c r="D11">
+        <v>1.1993355173053</v>
+      </c>
+      <c r="F11">
+        <v>35356</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.78470331600385035</v>
+      </c>
+      <c r="D12">
+        <v>1.8391119231548871</v>
+      </c>
+      <c r="F12">
+        <v>55420</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.78363015197400099</v>
+      </c>
+      <c r="D13">
+        <v>2.6013842370971876</v>
+      </c>
+      <c r="F13">
+        <v>66767</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.78333667892848402</v>
+      </c>
+      <c r="D14">
+        <v>2.929503635333957</v>
+      </c>
+      <c r="F14">
+        <v>81234</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.78277756500881845</v>
+      </c>
+      <c r="D15">
+        <v>3.8187444570018378</v>
+      </c>
+      <c r="F15">
+        <v>108281</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.78047088459262071</v>
+      </c>
+      <c r="D16">
+        <v>9.4569931269573964</v>
+      </c>
+      <c r="F16">
+        <v>154299</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.78003696743653761</v>
+      </c>
+      <c r="D17">
+        <v>12.513585954001949</v>
+      </c>
+      <c r="F17">
+        <v>143496</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.70587519535763132</v>
+      </c>
+      <c r="D2">
+        <v>4.6008798577686458E-2</v>
+      </c>
+      <c r="F2">
+        <v>5041</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.70227385866358794</v>
+      </c>
+      <c r="D3">
+        <v>5.2840324146882771E-2</v>
+      </c>
+      <c r="F3">
+        <v>6578</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.69719960936185199</v>
+      </c>
+      <c r="D4">
+        <v>6.9317985485954497E-2</v>
+      </c>
+      <c r="F4">
+        <v>4989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.69178432510737775</v>
+      </c>
+      <c r="D5">
+        <v>0.1104853179019082</v>
+      </c>
+      <c r="F5">
+        <v>7268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.68920036539657603</v>
+      </c>
+      <c r="D6">
+        <v>0.13939479474450642</v>
+      </c>
+      <c r="F6">
+        <v>7536</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.68542776617502355</v>
+      </c>
+      <c r="D7">
+        <v>0.19824986232592187</v>
+      </c>
+      <c r="F7">
+        <v>7531</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.6805500146494895</v>
+      </c>
+      <c r="D8">
+        <v>0.35840962458895054</v>
+      </c>
+      <c r="F8">
+        <v>11244</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.66242465517680149</v>
+      </c>
+      <c r="D9">
+        <v>1.2706501047780729</v>
+      </c>
+      <c r="F9">
+        <v>27589</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.66112477504929057</v>
+      </c>
+      <c r="D10">
+        <v>1.4160063871815278</v>
+      </c>
+      <c r="F10">
+        <v>21654</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.65916256446723753</v>
+      </c>
+      <c r="D11">
+        <v>1.7236606842079125</v>
+      </c>
+      <c r="F11">
+        <v>21335</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.65709059080619392</v>
+      </c>
+      <c r="D12">
+        <v>2.362723758521422</v>
+      </c>
+      <c r="F12">
+        <v>36068</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.6561365736225182</v>
+      </c>
+      <c r="D13">
+        <v>3.0596894666972148</v>
+      </c>
+      <c r="F13">
+        <v>65255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.65587626122791598</v>
+      </c>
+      <c r="D14">
+        <v>3.3526254372198681</v>
+      </c>
+      <c r="F14">
+        <v>58647</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.65550050184203157</v>
+      </c>
+      <c r="D15">
+        <v>3.9446100326940963</v>
+      </c>
+      <c r="F15">
+        <v>80206</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.65501353040903565</v>
+      </c>
+      <c r="D16">
+        <v>5.5099706579178429</v>
+      </c>
+      <c r="F16">
+        <v>126218</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.67914131221759788</v>
+      </c>
+      <c r="D17">
+        <v>13.537120516092093</v>
+      </c>
+      <c r="F17">
+        <v>211006</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.82262658718836357</v>
+      </c>
+      <c r="D2">
+        <v>4.0975202270888349E-2</v>
+      </c>
+      <c r="F2">
+        <v>7550</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.81867509008000305</v>
+      </c>
+      <c r="D3">
+        <v>4.8551071515263958E-2</v>
+      </c>
+      <c r="F3">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.81158857556007213</v>
+      </c>
+      <c r="D4">
+        <v>7.2080785028631592E-2</v>
+      </c>
+      <c r="F4">
+        <v>6898</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.80397075654035211</v>
+      </c>
+      <c r="D5">
+        <v>0.12869880929986505</v>
+      </c>
+      <c r="F5">
+        <v>9822</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.80154627146695512</v>
+      </c>
+      <c r="D6">
+        <v>0.15569366788217165</v>
+      </c>
+      <c r="F6">
+        <v>8849</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.79836657343020956</v>
+      </c>
+      <c r="D7">
+        <v>0.2053414713157701</v>
+      </c>
+      <c r="F7">
+        <v>10866</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.7902893512247553</v>
+      </c>
+      <c r="D8">
+        <v>0.50833957163223598</v>
+      </c>
+      <c r="F8">
+        <v>23612</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.77298714785462497</v>
+      </c>
+      <c r="D9">
+        <v>1.2211163754278158</v>
+      </c>
+      <c r="F9">
+        <v>42630</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.77196170722492885</v>
+      </c>
+      <c r="D10">
+        <v>1.3358861080212601</v>
+      </c>
+      <c r="F10">
+        <v>40815</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.77028436053313554</v>
+      </c>
+      <c r="D11">
+        <v>1.6002422875168762</v>
+      </c>
+      <c r="F11">
+        <v>36655</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.76812356852200536</v>
+      </c>
+      <c r="D12">
+        <v>2.2814354445873151</v>
+      </c>
+      <c r="F12">
+        <v>54084</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.76705997768645162</v>
+      </c>
+      <c r="D13">
+        <v>3.0300872622120858</v>
+      </c>
+      <c r="F13">
+        <v>75199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.76680966674475881</v>
+      </c>
+      <c r="D14">
+        <v>3.3096073394673131</v>
+      </c>
+      <c r="F14">
+        <v>89622</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.76640846689982944</v>
+      </c>
+      <c r="D15">
+        <v>3.9401317554964446</v>
+      </c>
+      <c r="F15">
+        <v>120588</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.76598677870022569</v>
+      </c>
+      <c r="D16">
+        <v>5.2527965129914742</v>
+      </c>
+      <c r="F16">
+        <v>145433</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.76584284251054968</v>
+      </c>
+      <c r="D17">
+        <v>6.3066581233910535</v>
+      </c>
+      <c r="F17">
+        <v>154799</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.81051721531386967</v>
+      </c>
+      <c r="D2">
+        <v>4.5905811733569647E-2</v>
+      </c>
+      <c r="F2">
+        <v>8639</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.80559905509303986</v>
+      </c>
+      <c r="D3">
+        <v>5.4681513474023814E-2</v>
+      </c>
+      <c r="F3">
+        <v>7755</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.79437071595311015</v>
+      </c>
+      <c r="D4">
+        <v>9.3095368370348777E-2</v>
+      </c>
+      <c r="F4">
+        <v>7756</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.78437739816785135</v>
+      </c>
+      <c r="D5">
+        <v>0.16401812657434703</v>
+      </c>
+      <c r="F5">
+        <v>9267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.78179824712783108</v>
+      </c>
+      <c r="D6">
+        <v>0.19286969182270219</v>
+      </c>
+      <c r="F6">
+        <v>9962</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.73861509557125093</v>
+      </c>
+      <c r="D7">
+        <v>0.64394155576003376</v>
+      </c>
+      <c r="F7">
+        <v>26035</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.7239276778497078</v>
+      </c>
+      <c r="D8">
+        <v>1.0957449909361878</v>
+      </c>
+      <c r="F8">
+        <v>28642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.71826449064591802</v>
+      </c>
+      <c r="D9">
+        <v>1.492769900300196</v>
+      </c>
+      <c r="F9">
+        <v>27254</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.7169209272600825</v>
+      </c>
+      <c r="D10">
+        <v>1.6428201800251401</v>
+      </c>
+      <c r="F10">
+        <v>46002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.71441221191838489</v>
+      </c>
+      <c r="D11">
+        <v>2.0411937649027232</v>
+      </c>
+      <c r="F11">
+        <v>59089</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.71140898708903821</v>
+      </c>
+      <c r="D12">
+        <v>3.0009007739958649</v>
+      </c>
+      <c r="F12">
+        <v>56005</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.71000249730629483</v>
+      </c>
+      <c r="D13">
+        <v>3.9926070186089171</v>
+      </c>
+      <c r="F13">
+        <v>64799</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.70963909730305796</v>
+      </c>
+      <c r="D14">
+        <v>4.3995195440660728</v>
+      </c>
+      <c r="F14">
+        <v>74053</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.70946135148915301</v>
+      </c>
+      <c r="D15">
+        <v>5.4266375647591136</v>
+      </c>
+      <c r="F15">
+        <v>32913</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.70938336809921632</v>
+      </c>
+      <c r="D16">
+        <v>7.4333965585710802</v>
+      </c>
+      <c r="F16">
+        <v>32823</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.70931978900076187</v>
+      </c>
+      <c r="D17">
+        <v>8.3607072135673963</v>
+      </c>
+      <c r="F17">
+        <v>19456</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -8374,14 +11953,310 @@
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S34" sqref="S34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.89989698283604536</v>
+      </c>
+      <c r="D2">
+        <v>3.155531600900717E-2</v>
+      </c>
+      <c r="F2">
+        <v>6961</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3">
+        <v>0.89647656261739816</v>
+      </c>
+      <c r="D3">
+        <v>3.853762450001523E-2</v>
+      </c>
+      <c r="F3">
+        <v>6564</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="C4">
+        <v>0.89037346242850812</v>
+      </c>
+      <c r="D4">
+        <v>5.8584318638587443E-2</v>
+      </c>
+      <c r="F4">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>0.88621163691614258</v>
+      </c>
+      <c r="D5">
+        <v>8.8697984884401171E-2</v>
+      </c>
+      <c r="F5">
+        <v>6516</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.08</v>
+      </c>
+      <c r="C6">
+        <v>0.8848203870098077</v>
+      </c>
+      <c r="D6">
+        <v>0.10430253083804066</v>
+      </c>
+      <c r="F6">
+        <v>6744</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="C7">
+        <v>0.88176045783105117</v>
+      </c>
+      <c r="D7">
+        <v>0.15325733618607895</v>
+      </c>
+      <c r="F7">
+        <v>9196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.02</v>
+      </c>
+      <c r="C8">
+        <v>0.87528208933887042</v>
+      </c>
+      <c r="D8">
+        <v>0.36502275913832838</v>
+      </c>
+      <c r="F8">
+        <v>13984</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="C9">
+        <v>0.86450820073480317</v>
+      </c>
+      <c r="D9">
+        <v>0.70402114128756377</v>
+      </c>
+      <c r="F9">
+        <v>30961</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C10">
+        <v>0.86375459887120343</v>
+      </c>
+      <c r="D10">
+        <v>0.78826607796981585</v>
+      </c>
+      <c r="F10">
+        <v>13434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C11">
+        <v>0.8622795572878329</v>
+      </c>
+      <c r="D11">
+        <v>1.0246497170621731</v>
+      </c>
+      <c r="F11">
+        <v>20732</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2E-3</v>
+      </c>
+      <c r="C12">
+        <v>0.86001109628141992</v>
+      </c>
+      <c r="D12">
+        <v>1.7172596556073976</v>
+      </c>
+      <c r="F12">
+        <v>56308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="C13">
+        <v>0.85929520098689671</v>
+      </c>
+      <c r="D13">
+        <v>2.2128180404941999</v>
+      </c>
+      <c r="F13">
+        <v>55502</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C14">
+        <v>0.85914572259899691</v>
+      </c>
+      <c r="D14">
+        <v>2.3798224972637114</v>
+      </c>
+      <c r="F14">
+        <v>70100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>0.85883863360350332</v>
+      </c>
+      <c r="D15">
+        <v>2.8717284192911463</v>
+      </c>
+      <c r="F15">
+        <v>66371</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C16">
+        <v>0.8583150789549352</v>
+      </c>
+      <c r="D16">
+        <v>4.6092782479164836</v>
+      </c>
+      <c r="F16">
+        <v>94877</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="3">
+        <v>1E-4</v>
+      </c>
+      <c r="C17">
+        <v>0.85765747974689188</v>
+      </c>
+      <c r="D17">
+        <v>9.0752577575214683</v>
+      </c>
+      <c r="F17">
+        <v>116049</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
fix key to runs
</commit_message>
<xml_diff>
--- a/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
+++ b/data/Summer2017/L-curve/compiled_L-curve_data_2017-06-21_updated.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\L-curve_Analysis_Summer-2017\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="6315" windowHeight="9015" tabRatio="851"/>
   </bookViews>
@@ -568,7 +573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -576,9 +581,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:B40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -675,7 +685,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>25</v>
@@ -683,7 +693,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>24</v>
@@ -906,8 +916,13 @@
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup scale="86" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;F</oddHeader>
+    <oddFooter>&amp;A</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>